<commit_message>
jap mockup done backend done sekarang lanjut integrasi front end dengan backend
</commit_message>
<xml_diff>
--- a/database schema.xlsx
+++ b/database schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hacktiv8\Phase 2 Redone\Portfolio\e-commerce-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68140D2E-4743-4345-BFB6-4F4BDD4A4978}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E382FD84-A046-4146-B5A5-FC306526EDB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{FAE0166B-18A7-48EC-9FB1-7CF99801D0C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{FAE0166B-18A7-48EC-9FB1-7CF99801D0C4}"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="3" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="transaction" sheetId="2" r:id="rId3"/>
     <sheet name="cart" sheetId="1" r:id="rId4"/>
     <sheet name="componentSchema" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="143">
   <si>
     <t>CartId</t>
   </si>
@@ -466,6 +467,48 @@
   </si>
   <si>
     <t>incomplete</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
+    <t>banner</t>
+  </si>
+  <si>
+    <t>card small</t>
+  </si>
+  <si>
+    <t>product search Page</t>
+  </si>
+  <si>
+    <t>user login page</t>
+  </si>
+  <si>
+    <t>user register page</t>
+  </si>
+  <si>
+    <t>view cart page</t>
+  </si>
+  <si>
+    <t>individual product page</t>
+  </si>
+  <si>
+    <t>item you sell</t>
+  </si>
+  <si>
+    <t>per seller item sold</t>
+  </si>
+  <si>
+    <t>cardSmall</t>
+  </si>
+  <si>
+    <t>transactionForm</t>
+  </si>
+  <si>
+    <t>product info</t>
+  </si>
+  <si>
+    <t>user form</t>
   </si>
 </sst>
 </file>
@@ -1033,19 +1076,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9AF392A-B338-461B-9073-64352BEA8411}">
   <dimension ref="A3:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="12.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="12.44140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="5" width="12.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>45</v>
       </c>
@@ -1074,7 +1117,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
@@ -1103,7 +1146,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>46</v>
       </c>
@@ -1132,7 +1175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -1143,7 +1186,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1154,7 +1197,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1165,7 +1208,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1176,7 +1219,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1204,15 +1247,15 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="4" width="15" customWidth="1"/>
     <col min="5" max="6" width="15" style="14" customWidth="1"/>
     <col min="7" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1224,7 +1267,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1236,7 +1279,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>45</v>
       </c>
@@ -1266,7 +1309,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>51</v>
       </c>
@@ -1296,7 +1339,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>52</v>
       </c>
@@ -1326,7 +1369,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>53</v>
       </c>
@@ -1356,7 +1399,7 @@
       </c>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>54</v>
       </c>
@@ -1386,7 +1429,7 @@
       </c>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1398,7 +1441,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1410,7 +1453,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="20.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1422,7 +1465,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1434,7 +1477,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1446,7 +1489,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1458,7 +1501,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1470,7 +1513,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1495,39 +1538,39 @@
       <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="16.109375" customWidth="1"/>
-    <col min="6" max="7" width="16.109375" style="20" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
+    <col min="1" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="7" width="16.140625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F1" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F2" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H5" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H6" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H7" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -1553,7 +1596,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>56</v>
       </c>
@@ -1580,7 +1623,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>57</v>
       </c>
@@ -1605,7 +1648,7 @@
       </c>
       <c r="H10" s="21"/>
     </row>
-    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -1615,7 +1658,7 @@
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
     </row>
-    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>58</v>
       </c>
@@ -1640,7 +1683,7 @@
       </c>
       <c r="H12" s="21"/>
     </row>
-    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>59</v>
       </c>
@@ -1665,7 +1708,7 @@
       </c>
       <c r="H13" s="21"/>
     </row>
-    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
@@ -1675,7 +1718,7 @@
       <c r="G14" s="23"/>
       <c r="H14" s="23"/>
     </row>
-    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>60</v>
       </c>
@@ -1700,7 +1743,7 @@
       </c>
       <c r="H15" s="21"/>
     </row>
-    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>61</v>
       </c>
@@ -1725,7 +1768,7 @@
       </c>
       <c r="H16" s="21"/>
     </row>
-    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>62</v>
       </c>
@@ -1750,7 +1793,7 @@
       </c>
       <c r="H17" s="21"/>
     </row>
-    <row r="18" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>63</v>
       </c>
@@ -1789,26 +1832,26 @@
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.33203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="13.44140625" style="1" customWidth="1"/>
-    <col min="4" max="6" width="13.44140625" style="18" customWidth="1"/>
-    <col min="7" max="9" width="13.44140625" style="19" customWidth="1"/>
-    <col min="10" max="11" width="13.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.44140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.88671875" style="1"/>
-    <col min="18" max="18" width="27.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="2.28515625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4" max="6" width="13.42578125" style="18" customWidth="1"/>
+    <col min="7" max="9" width="13.42578125" style="19" customWidth="1"/>
+    <col min="10" max="11" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" style="1"/>
+    <col min="18" max="18" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J2" s="7"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P4" s="1" t="s">
         <v>84</v>
       </c>
@@ -1819,7 +1862,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="2:18" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="7"/>
       <c r="O5" s="26" t="s">
         <v>76</v>
@@ -1829,7 +1872,7 @@
       </c>
       <c r="R5" s="5"/>
     </row>
-    <row r="6" spans="2:18" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="7"/>
       <c r="O6" s="26" t="s">
         <v>77</v>
@@ -1844,7 +1887,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="2:18" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="7"/>
       <c r="O7" s="26" t="s">
         <v>78</v>
@@ -1859,7 +1902,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="7"/>
       <c r="O8" s="26" t="s">
         <v>14</v>
@@ -1872,7 +1915,7 @@
       </c>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="2:18" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" s="7"/>
       <c r="K9" s="1" t="s">
         <v>11</v>
@@ -1896,7 +1939,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="2:18" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="7"/>
       <c r="K10" s="1" t="s">
         <v>80</v>
@@ -1915,7 +1958,7 @@
       </c>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C11" s="7" t="s">
         <v>64</v>
       </c>
@@ -1935,7 +1978,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="2:18" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>0</v>
       </c>
@@ -1979,7 +2022,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>1</v>
       </c>
@@ -2024,7 +2067,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:18" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:18" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="31"/>
       <c r="C14" s="31" t="s">
         <v>57</v>
@@ -2054,7 +2097,7 @@
       <c r="N14" s="31"/>
       <c r="O14" s="33"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -2070,7 +2113,7 @@
       <c r="N15" s="22"/>
       <c r="O15" s="27"/>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>71</v>
       </c>
@@ -2113,7 +2156,7 @@
       </c>
       <c r="O16" s="26"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
         <v>59</v>
@@ -2143,7 +2186,7 @@
       <c r="N17" s="5"/>
       <c r="O17" s="26"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
@@ -2159,7 +2202,7 @@
       <c r="N18" s="22"/>
       <c r="O18" s="27"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>72</v>
       </c>
@@ -2200,7 +2243,7 @@
       <c r="N19" s="5"/>
       <c r="O19" s="26"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
         <v>61</v>
@@ -2230,7 +2273,7 @@
       <c r="N20" s="5"/>
       <c r="O20" s="26"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
         <v>62</v>
@@ -2260,7 +2303,7 @@
       <c r="N21" s="5"/>
       <c r="O21" s="26"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
         <v>63</v>
@@ -2290,22 +2333,22 @@
       <c r="N22" s="5"/>
       <c r="O22" s="26"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="37" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K25" s="35" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K26" s="36" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K28" s="37" t="s">
         <v>127</v>
       </c>
@@ -2321,29 +2364,29 @@
   <dimension ref="D1:Q22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:J12"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.88671875" style="1"/>
+    <col min="1" max="4" width="8.85546875" style="1"/>
     <col min="5" max="5" width="3" style="28" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" style="28" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3" style="28" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3" style="28" customWidth="1"/>
-    <col min="12" max="12" width="8.88671875" style="1"/>
-    <col min="13" max="13" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="8.88671875" style="1"/>
-    <col min="17" max="17" width="24.5546875" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="8.85546875" style="1"/>
+    <col min="13" max="13" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" style="1"/>
+    <col min="17" max="17" width="24.5703125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:17" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="4:17" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="30" t="s">
@@ -2361,7 +2404,7 @@
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
     </row>
-    <row r="2" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="4:17" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>94</v>
       </c>
@@ -2372,7 +2415,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F4" s="29"/>
       <c r="G4" s="29"/>
       <c r="H4" s="29"/>
@@ -2386,7 +2429,7 @@
       <c r="P4" s="29"/>
       <c r="Q4" s="29"/>
     </row>
-    <row r="5" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F5" s="1" t="s">
         <v>106</v>
       </c>
@@ -2394,12 +2437,12 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F6" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H7" s="29"/>
       <c r="I7" s="29"/>
       <c r="J7" s="29"/>
@@ -2411,7 +2454,7 @@
       <c r="P7" s="29"/>
       <c r="Q7" s="29"/>
     </row>
-    <row r="8" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H8" s="1" t="s">
         <v>122</v>
       </c>
@@ -2419,7 +2462,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="10" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H10" s="29"/>
       <c r="I10" s="29"/>
       <c r="J10" s="29"/>
@@ -2431,7 +2474,7 @@
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
     </row>
-    <row r="11" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H11" s="1" t="s">
         <v>96</v>
       </c>
@@ -2446,10 +2489,10 @@
       </c>
       <c r="Q11" s="24"/>
     </row>
-    <row r="12" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:17" x14ac:dyDescent="0.25">
       <c r="Q12" s="24"/>
     </row>
-    <row r="13" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:17" x14ac:dyDescent="0.25">
       <c r="H13" s="29"/>
       <c r="I13" s="29"/>
       <c r="J13" s="29"/>
@@ -2461,7 +2504,7 @@
       <c r="P13" s="29"/>
       <c r="Q13" s="29"/>
     </row>
-    <row r="14" spans="4:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:17" ht="45" x14ac:dyDescent="0.25">
       <c r="H14" s="1" t="s">
         <v>123</v>
       </c>
@@ -2487,7 +2530,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F15" s="29"/>
       <c r="G15" s="29"/>
       <c r="H15" s="29"/>
@@ -2501,7 +2544,7 @@
       <c r="P15" s="29"/>
       <c r="Q15" s="29"/>
     </row>
-    <row r="16" spans="4:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:17" x14ac:dyDescent="0.25">
       <c r="F16" s="1" t="s">
         <v>111</v>
       </c>
@@ -2518,12 +2561,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="6:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:17" x14ac:dyDescent="0.25">
       <c r="F17" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="6:17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H19" s="1" t="s">
         <v>96</v>
       </c>
@@ -2540,7 +2583,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="6:17" ht="72" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:17" ht="45" x14ac:dyDescent="0.25">
       <c r="H22" s="1" t="s">
         <v>123</v>
       </c>
@@ -2564,6 +2607,111 @@
       </c>
       <c r="Q22" s="24" t="s">
         <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53CCC7B9-01D6-4EE5-8718-63ECBE7ECB7E}">
+  <dimension ref="D3:K39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="4" style="28" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4" style="28" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" style="28" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="4" style="28" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F10" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="F14" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F28" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F32" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F35" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>